<commit_message>
rerun analysis up to HGLAC
</commit_message>
<xml_diff>
--- a/results_summary_table.xlsx
+++ b/results_summary_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\KBS_ladybeetles_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A818E2C5-8D1B-4850-93DF-19C26D5935DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9AB678-824B-42E4-BC52-A259574FBCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FC4A10F-598C-48DF-BC58-E45CC3EDA496}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>Species</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Is there an overall increase/decrease in the last 10 years?</t>
-  </si>
-  <si>
-    <t>Detection frequency (1993-1998: 2015-2020)</t>
   </si>
   <si>
     <t>Adalia bipunctata</t>
@@ -163,6 +160,189 @@
   </si>
   <si>
     <t>5:5</t>
+  </si>
+  <si>
+    <t>Edf=3.837, GCV=15.401 Very strong temporal dependency, very cyclic looking overall pattern</t>
+  </si>
+  <si>
+    <t>GCV=14.293</t>
+  </si>
+  <si>
+    <t>GCV=14.007,  Pattern varies by crop type, with significant temporal variability only observed in annual crop plots</t>
+  </si>
+  <si>
+    <t>-0.013+/-0.003</t>
+  </si>
+  <si>
+    <t>-0.005+/-0.001</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Edf=2.660
+GCV=1.0754, still present but trend suggests loss occurring around early 2000s and no real recovery</t>
+  </si>
+  <si>
+    <t>GCV=0.89478 Strong crop dependency in pattern. Temporal structure in all perennial crops deciduous and successional forest, all decline patterns to about 2000, then stability, trends are stable (occasional rare occurrence) in other plots</t>
+  </si>
+  <si>
+    <t>GCV=0.99115</t>
+  </si>
+  <si>
+    <t>-0.0049+/-0.00008</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>5:4</t>
+  </si>
+  <si>
+    <t>NS GAM</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>GCV=0.19632 Very rare in all forests, no temporal structure,  slight decline over time observed in alfalfa, conventional, early successional and poplar plots, but essentially explained by difference of occasional rare captures going to zero</t>
+  </si>
+  <si>
+    <t>GCV=0.20391</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>-0.00008+/-0.00001</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>5:0</t>
+  </si>
+  <si>
+    <t>Edf= 1.553, GCV=0.20844 Temporal structure suggests decrease from rare to non-existent. Has been relatively rare since beginning of study, with a handful of individuals captured across site each year, but has not been seen since 2008</t>
+  </si>
+  <si>
+    <t>Species is rare at site, was removed from data sheet from 2005-2013</t>
+  </si>
+  <si>
+    <t>Species relatively rare at site, removed from data sheet 2004-2008</t>
+  </si>
+  <si>
+    <t>Edf=2.334, GCV=0.8658
+Abundance peaks around 2000, then declines to occasional observations after 2010, not reported in 2004-2014 in forest plots</t>
+  </si>
+  <si>
+    <t>GCV=0.84666
+Idiosyncratic structure within individual plant communities, but all follow general peaked distribution through time</t>
+  </si>
+  <si>
+    <t>Edf=3.288, GCV=1.7499, fairly consistently common through most of study period,  with a trough between 2000 and 2012, but apparent steep decline in recent years of study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Was not monitored in forest plots 2004-2011</t>
+  </si>
+  <si>
+    <t>GCV=1.7292
+Annual and perennial crops follow same temporal pattern, with a sharper decline in annual plots in recent years, but no temporal structure within fores</t>
+  </si>
+  <si>
+    <t>GCV=2.3836
+No significant temporal structure in forests- rarely captured in these plots, strongly peaked distribution in annual crops, curve is similar shape but smoother in perennial crops</t>
+  </si>
+  <si>
+    <t>Edf=2.556, GCV=2.5377
+Significant temporal structure. First detected at site in 2000, increased until 2013, then declines</t>
+  </si>
+  <si>
+    <t>Edf= 1.954, GCV=4.9521
+Species was first captured in 2007, and has a significant peaked temporal structure. Increased from 2007-2014 and then declined.</t>
+  </si>
+  <si>
+    <t>GCV=4.7016
+No significant temporal structure in any plot but early successional, where this species in most common.</t>
+  </si>
+  <si>
+    <t>Edf=3.497, GCV=3.2699 Decreasing trend which stabilized in mid-2000s, increase 2010-2015, but then rapid drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCV=3.0805 Relatively stable in all plant communities but poplar trees, this dynamic drives the pattern observed in the overall dataset.
+</t>
+  </si>
+  <si>
+    <t>GCV=3.187</t>
+  </si>
+  <si>
+    <t>-0.002+/-0.001</t>
+  </si>
+  <si>
+    <t>-0.0007+/-0.0002</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edf=1.106, GCV=0.1417, no significant temporal structure. </t>
+  </si>
+  <si>
+    <t>GCV=0.13216, decrease in conventional plots, increase in early successional, but trends are based on very limited observations (single individuals per year)</t>
+  </si>
+  <si>
+    <t>GCV=0.13862</t>
+  </si>
+  <si>
+    <t>1:3</t>
+  </si>
+  <si>
+    <t>Edf=3.84, GCV=7.94, strong temporal structure. Increasing after invasion to ~2000, then largely stable, then precipitous decline with infection point near 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCV=7.3388
+No temporal structure observed in individual forest types. All other plant communities with idiosyncratic temporal structure but most generally follow general domed pattern with recent decline, except in poplar
+</t>
+  </si>
+  <si>
+    <t>GCV=7.3743</t>
+  </si>
+  <si>
+    <t>-0.026+/-0.003</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>4:5</t>
+  </si>
+  <si>
+    <t>Detection frequency (1993-1997: 2016-2020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edf=2.051, GCV=0.88359, no apparent temporal structure. </t>
+  </si>
+  <si>
+    <t>GCV=0.85873
+Temporal structure in early successional (overall increase) and organic plots (overall decrease) seems to be driven by a few rare observations.</t>
+  </si>
+  <si>
+    <t>GCV=0.88574</t>
+  </si>
+  <si>
+    <t>-0.0009+/-0.0002</t>
+  </si>
+  <si>
+    <t>4:2</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
 </sst>
 </file>
@@ -520,10 +700,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CCDAD8-85EA-475F-A624-C016D6A09759}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,25 +715,25 @@
     <col min="2" max="2" width="28.6328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="31.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="25.90625" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.90625" style="2" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -562,152 +745,359 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="174" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="174" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="261" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="188" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="232" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
+      <c r="D15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete individual species analysis
</commit_message>
<xml_diff>
--- a/results_summary_table.xlsx
+++ b/results_summary_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\KBS_ladybeetles_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9AB678-824B-42E4-BC52-A259574FBCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CEDC97-B2A2-4FE0-AC0C-A3783B00E6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FC4A10F-598C-48DF-BC58-E45CC3EDA496}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
   <si>
     <t>Species</t>
   </si>
@@ -202,9 +202,6 @@
     <t>5:4</t>
   </si>
   <si>
-    <t>NS GAM</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -238,38 +235,7 @@
     <t>Species relatively rare at site, removed from data sheet 2004-2008</t>
   </si>
   <si>
-    <t>Edf=2.334, GCV=0.8658
-Abundance peaks around 2000, then declines to occasional observations after 2010, not reported in 2004-2014 in forest plots</t>
-  </si>
-  <si>
-    <t>GCV=0.84666
-Idiosyncratic structure within individual plant communities, but all follow general peaked distribution through time</t>
-  </si>
-  <si>
-    <t>Edf=3.288, GCV=1.7499, fairly consistently common through most of study period,  with a trough between 2000 and 2012, but apparent steep decline in recent years of study.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Was not monitored in forest plots 2004-2011</t>
-  </si>
-  <si>
-    <t>GCV=1.7292
-Annual and perennial crops follow same temporal pattern, with a sharper decline in annual plots in recent years, but no temporal structure within fores</t>
-  </si>
-  <si>
-    <t>GCV=2.3836
-No significant temporal structure in forests- rarely captured in these plots, strongly peaked distribution in annual crops, curve is similar shape but smoother in perennial crops</t>
-  </si>
-  <si>
-    <t>Edf=2.556, GCV=2.5377
-Significant temporal structure. First detected at site in 2000, increased until 2013, then declines</t>
-  </si>
-  <si>
-    <t>Edf= 1.954, GCV=4.9521
-Species was first captured in 2007, and has a significant peaked temporal structure. Increased from 2007-2014 and then declined.</t>
-  </si>
-  <si>
-    <t>GCV=4.7016
-No significant temporal structure in any plot but early successional, where this species in most common.</t>
   </si>
   <si>
     <t>Edf=3.497, GCV=3.2699 Decreasing trend which stabilized in mid-2000s, increase 2010-2015, but then rapid drop</t>
@@ -343,6 +309,88 @@
   </si>
   <si>
     <t>2017</t>
+  </si>
+  <si>
+    <t>not reported in 2004-2014 in forest plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edf=2.338, GCV=0.86592
+Abundance peaks around 2000, then declines to occasional observations after 2010 </t>
+  </si>
+  <si>
+    <t>GCV=0.84722
+Idiosyncratic structure within individual plant communities, but all follow general peaked distribution through time</t>
+  </si>
+  <si>
+    <t>GCV=0.87579</t>
+  </si>
+  <si>
+    <t>-0.00048+/-0.00006</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>4:3</t>
+  </si>
+  <si>
+    <t>Edf=3.292, GCV=1.7508, fairly consistently common through most of study period,  with a trough between 2000 and 2012, but apparent steep decline in recent years of study.</t>
+  </si>
+  <si>
+    <t>GCV=1.7731</t>
+  </si>
+  <si>
+    <t>GCV=1.7326
+Annual and perennial crops follow same temporal pattern, with a sharper decline in annual plots in recent years, but no temporal structure within forest</t>
+  </si>
+  <si>
+    <t>-0.0031+/-0.0006</t>
+  </si>
+  <si>
+    <t>-0.0005+/-0.0001</t>
+  </si>
+  <si>
+    <t>First recorded in 1994</t>
+  </si>
+  <si>
+    <t>NS GAM, Species was added to the survey in 2004</t>
+  </si>
+  <si>
+    <t>Edf=2.559, GCV=2.550
+Significant temporal structure. First detected at site in 2000, increased until 2013, then declines</t>
+  </si>
+  <si>
+    <t>Species first added to survey in 1999, no data in 2004</t>
+  </si>
+  <si>
+    <t>GCV=2.4243</t>
+  </si>
+  <si>
+    <t>GCV=2.395
+No significant temporal structure in forests- rarely captured in these plots, strongly peaked distribution in annual crops, curve is similar shape but smoother in perennial crops</t>
+  </si>
+  <si>
+    <t>-0.004+/-0.001</t>
+  </si>
+  <si>
+    <t>0.0014+/-0.0003</t>
+  </si>
+  <si>
+    <t>Species first recorded in survey in 2007</t>
+  </si>
+  <si>
+    <t>Edf= 1.955, GCV=4.9967
+Has a significant peaked temporal structure. Increased from 2007-2014 and then declined.</t>
+  </si>
+  <si>
+    <t>GCV=4.7464
+No significant temporal structure in any plot but early successional, where this species in most common.</t>
+  </si>
+  <si>
+    <t>GCV=4.8405</t>
+  </si>
+  <si>
+    <t>0.0022+/-0.0008</t>
   </si>
 </sst>
 </file>
@@ -703,10 +751,10 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,13 +793,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -783,7 +831,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -812,7 +860,7 @@
         <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="174" x14ac:dyDescent="0.35">
@@ -907,28 +955,28 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="188" customHeight="1" x14ac:dyDescent="0.35">
@@ -936,22 +984,22 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>53</v>
@@ -965,31 +1013,31 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="232" x14ac:dyDescent="0.35">
@@ -997,28 +1045,31 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
@@ -1026,78 +1077,159 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>96</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>98</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>103</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>74</v>
+        <v>111</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate some summary stats
</commit_message>
<xml_diff>
--- a/results_summary_table.xlsx
+++ b/results_summary_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\KBS_ladybeetles_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CEDC97-B2A2-4FE0-AC0C-A3783B00E6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F789BA-4096-4C17-9E92-5B69128FCDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FC4A10F-598C-48DF-BC58-E45CC3EDA496}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="186">
   <si>
     <t>Species</t>
   </si>
@@ -391,12 +391,231 @@
   </si>
   <si>
     <t>0.0022+/-0.0008</t>
+  </si>
+  <si>
+    <t>Native species</t>
+  </si>
+  <si>
+    <t>Invasive species</t>
+  </si>
+  <si>
+    <t>Total community</t>
+  </si>
+  <si>
+    <t>Predation potential</t>
+  </si>
+  <si>
+    <t>Edf=3.892, GCV=13.289 Two peaks over time- increase to 1999 then strong drop troughing near 2008, peak again near 2015 then drop, but overall deacreasing</t>
+  </si>
+  <si>
+    <t>GCV=12.39</t>
+  </si>
+  <si>
+    <t>GCV=12.194 No temporal structure in forests, two peaks over time in annual and perrenial crops, with pattern more pronounced in annual systems.</t>
+  </si>
+  <si>
+    <t>-0.018+/-0.003</t>
+  </si>
+  <si>
+    <t>-0.007+/-0.001</t>
+  </si>
+  <si>
+    <t>Edf=3.968, GCV=20.178 Single peaked distribution over time, peaking near 2007</t>
+  </si>
+  <si>
+    <t>GCV=19.684</t>
+  </si>
+  <si>
+    <t>GCV=19.681,  variable patterns across all crops, no temporal variability detected in any forests</t>
+  </si>
+  <si>
+    <t>-0.030+/-0.005</t>
+  </si>
+  <si>
+    <t>-0.007+/-0.002</t>
+  </si>
+  <si>
+    <t>Edf=3.975, GCV=21.237,  increase until 2000, then declining at variable rates for last 20 years with steepest decline in last 5 years</t>
+  </si>
+  <si>
+    <t>GCV=20.678</t>
+  </si>
+  <si>
+    <t>GCV=20.574 No trends within forest, but domed distribution through time in annual and perrenial croplands, steep decline in annuals in later part of study period</t>
+  </si>
+  <si>
+    <t>-0.048+/-0.007</t>
+  </si>
+  <si>
+    <t>-0.014+/-0.002</t>
+  </si>
+  <si>
+    <t>Edf=3.955, GCV=12.049, domed distribution thrrough time increasing to 2001-2002 and decreasing after</t>
+  </si>
+  <si>
+    <t>GCV=11.672</t>
+  </si>
+  <si>
+    <t>GCV=11.625, significant and variable temporal structure within all croplands, but most domed with recent decline, except within poplar</t>
+  </si>
+  <si>
+    <t>-0.025+/-0.003</t>
+  </si>
+  <si>
+    <t>-0.009+/-0.001</t>
+  </si>
+  <si>
+    <t>Avg per trap</t>
+  </si>
+  <si>
+    <t>0.430</t>
+  </si>
+  <si>
+    <t>0.00162</t>
+  </si>
+  <si>
+    <t>0.0116</t>
+  </si>
+  <si>
+    <t>0.317</t>
+  </si>
+  <si>
+    <t>0.124</t>
+  </si>
+  <si>
+    <t>0.00668</t>
+  </si>
+  <si>
+    <t>0.000806</t>
+  </si>
+  <si>
+    <t>0.0291</t>
+  </si>
+  <si>
+    <t>0.000380</t>
+  </si>
+  <si>
+    <t>0.234</t>
+  </si>
+  <si>
+    <t>0.00347</t>
+  </si>
+  <si>
+    <t>0.00562</t>
+  </si>
+  <si>
+    <t>0.0181</t>
+  </si>
+  <si>
+    <t>0.0221</t>
+  </si>
+  <si>
+    <t>0.0581</t>
+  </si>
+  <si>
+    <t>0.192</t>
+  </si>
+  <si>
+    <t>0.596</t>
+  </si>
+  <si>
+    <t>0.788</t>
+  </si>
+  <si>
+    <t>-0.00013</t>
+  </si>
+  <si>
+    <t>-0.012</t>
+  </si>
+  <si>
+    <t>-0.005</t>
+  </si>
+  <si>
+    <t>-0.0049</t>
+  </si>
+  <si>
+    <t>-0.00008</t>
+  </si>
+  <si>
+    <t>-0.0007</t>
+  </si>
+  <si>
+    <t>-0.00048</t>
+  </si>
+  <si>
+    <t>-0.0005</t>
+  </si>
+  <si>
+    <t>0.0014</t>
+  </si>
+  <si>
+    <t>0.0022</t>
+  </si>
+  <si>
+    <t>-0.007</t>
+  </si>
+  <si>
+    <t>-0.014</t>
+  </si>
+  <si>
+    <t>-0.009</t>
+  </si>
+  <si>
+    <t>raw slope net</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>net % change per year</t>
+  </si>
+  <si>
+    <t>raw slope last 10</t>
+  </si>
+  <si>
+    <t>% change per year last 10</t>
+  </si>
+  <si>
+    <t>-0.00014</t>
+  </si>
+  <si>
+    <t>-0.013</t>
+  </si>
+  <si>
+    <t>-0.002</t>
+  </si>
+  <si>
+    <t>-0.026</t>
+  </si>
+  <si>
+    <t>-0.0009</t>
+  </si>
+  <si>
+    <t>-0.0031</t>
+  </si>
+  <si>
+    <t>-0.004</t>
+  </si>
+  <si>
+    <t>-0.018</t>
+  </si>
+  <si>
+    <t>-0.030</t>
+  </si>
+  <si>
+    <t>-0.048</t>
+  </si>
+  <si>
+    <t>-0.025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,12 +645,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -748,491 +973,935 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CCDAD8-85EA-475F-A624-C016D6A09759}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.90625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.90625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" style="2" customWidth="1"/>
+    <col min="11" max="12" width="15.81640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.90625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="4">
+        <f>100*E2/B2</f>
+        <v>-1.7766497461928934</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L2" s="3">
+        <f>100*K2/B2</f>
+        <v>-6.0913705583756341</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="4">
+        <f>100*E3/B3</f>
+        <v>-1.1744966442953022</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L3" s="3">
+        <f>100*K3/B3</f>
+        <v>-5.0335570469798663</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="4">
+        <f>100*E4/B4</f>
+        <v>-2.0930232558139532</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="L4" s="3">
+        <f>100*K4/B4</f>
+        <v>-5.8139534883720927</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="4">
+        <f>100*E5/B5</f>
+        <v>-3.7854889589905363</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="3">
+        <f>100*K5/B5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="232" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="4">
+        <f>100*E6/B6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="L6" s="3">
+        <f>100*K6/B6</f>
+        <v>-11.111111111111111</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="4">
+        <f>100*E7/B7</f>
+        <v>-3.6458333333333335</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="L7" s="3">
+        <f>100*K7/B7</f>
+        <v>-9.3749999999999982</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="188" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="4">
+        <f>100*E8/B8</f>
+        <v>-4.032258064516129</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L8" s="3">
+        <f>100*K8/B8</f>
+        <v>-10.483870967741936</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="169" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="4">
+        <f>100*E9/B9</f>
+        <v>3.7865748709122204</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L9" s="3">
+        <f>100*K9/B9</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="4">
+        <f>100*E10/B10</f>
+        <v>-2.4054982817869415</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L10" s="3">
+        <f>100*K10/B10</f>
+        <v>-6.8728522336769764</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="116" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="4">
+        <f>100*E11/B11</f>
+        <v>6.3348416289592748</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L11" s="3">
+        <f>100*K11/B11</f>
+        <v>-18.099547511312217</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="116" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="4">
+        <f>100*E12/B12</f>
+        <v>-2.7624309392265194</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" s="3">
+        <f>100*K12/B12</f>
+        <v>-17.127071823204417</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="4">
+        <f>100*E13/B13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="3">
+        <f>100*K13/B13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="232" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="4">
+        <f>100*E14/B14</f>
+        <v>-73.353293413173645</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" s="3">
+        <f>100*K14/B14</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="4">
+        <f>100*E15/B15</f>
+        <v>-8.5409252669039155</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L15" s="3">
+        <f>100*K15/B15</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="4">
+        <f>100*E16/B16</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L16" s="3">
+        <f>100*K16/B16</f>
+        <v>-25.936599423631122</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="2">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E17" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="4">
+        <f>100*E17/B17</f>
+        <v>-8.0246913580246915</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K17" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="L17" s="3">
+        <f>100*K17/B17</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2">
+      <c r="N17" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="18" spans="1:15" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" s="4">
+        <f>100*E18/B18</f>
+        <v>-9.9255583126550881</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L18" s="3">
+        <f>100*K18/B18</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="E19" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="4">
+        <f>100*E19/B19</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="K19" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L19" s="3">
+        <f>100*K19/B19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="174" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="261" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="188" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="O19" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="232" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
+    <sortCondition descending="1" ref="B2:B21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
oh, crap- did a lot. added new segmented analyisis
</commit_message>
<xml_diff>
--- a/results_summary_table.xlsx
+++ b/results_summary_table.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\KBS_ladybeetles_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F789BA-4096-4C17-9E92-5B69128FCDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FEDAE5-4556-4163-8BFB-2A33A7AB4FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FC4A10F-598C-48DF-BC58-E45CC3EDA496}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6FC4A10F-598C-48DF-BC58-E45CC3EDA496}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="aggregated data" sheetId="2" r:id="rId2"/>
+    <sheet name="Single species" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="189">
   <si>
     <t>Species</t>
   </si>
@@ -607,6 +610,15 @@
   </si>
   <si>
     <t>-0.025</t>
+  </si>
+  <si>
+    <t>GCV=19.684, Patterns largely track overall trends, except stabilization in annual crops in most recent 5 years.</t>
+  </si>
+  <si>
+    <t>GCV=11.672, patterns largely track overall abundance</t>
+  </si>
+  <si>
+    <t>Colum h on, into table 2</t>
   </si>
 </sst>
 </file>
@@ -616,8 +628,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -645,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -659,6 +679,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,11 +1008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CCDAD8-85EA-475F-A624-C016D6A09759}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="A1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,7 +1096,7 @@
         <v>168</v>
       </c>
       <c r="F2" s="4">
-        <f>100*E2/B2</f>
+        <f t="shared" ref="F2:F19" si="0">100*E2/B2</f>
         <v>-1.7766497461928934</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1082,7 +1115,7 @@
         <v>184</v>
       </c>
       <c r="L2" s="3">
-        <f>100*K2/B2</f>
+        <f t="shared" ref="L2:L19" si="1">100*K2/B2</f>
         <v>-6.0913705583756341</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -1109,7 +1142,7 @@
         <v>167</v>
       </c>
       <c r="F3" s="4">
-        <f>100*E3/B3</f>
+        <f t="shared" si="0"/>
         <v>-1.1744966442953022</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1128,7 +1161,7 @@
         <v>183</v>
       </c>
       <c r="L3" s="3">
-        <f>100*K3/B3</f>
+        <f t="shared" si="1"/>
         <v>-5.0335570469798663</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1155,7 +1188,7 @@
         <v>169</v>
       </c>
       <c r="F4" s="4">
-        <f>100*E4/B4</f>
+        <f t="shared" si="0"/>
         <v>-2.0930232558139532</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1174,7 +1207,7 @@
         <v>185</v>
       </c>
       <c r="L4" s="3">
-        <f>100*K4/B4</f>
+        <f t="shared" si="1"/>
         <v>-5.8139534883720927</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1201,7 +1234,7 @@
         <v>158</v>
       </c>
       <c r="F5" s="4">
-        <f>100*E5/B5</f>
+        <f t="shared" si="0"/>
         <v>-3.7854889589905363</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1220,7 +1253,7 @@
         <v>171</v>
       </c>
       <c r="L5" s="3">
-        <f>100*K5/B5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1247,7 +1280,7 @@
         <v>171</v>
       </c>
       <c r="F6" s="4">
-        <f>100*E6/B6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1266,7 +1299,7 @@
         <v>178</v>
       </c>
       <c r="L6" s="3">
-        <f>100*K6/B6</f>
+        <f t="shared" si="1"/>
         <v>-11.111111111111111</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1296,7 +1329,7 @@
         <v>167</v>
       </c>
       <c r="F7" s="4">
-        <f>100*E7/B7</f>
+        <f t="shared" si="0"/>
         <v>-3.6458333333333335</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1315,7 +1348,7 @@
         <v>182</v>
       </c>
       <c r="L7" s="3">
-        <f>100*K7/B7</f>
+        <f t="shared" si="1"/>
         <v>-9.3749999999999982</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1342,7 +1375,7 @@
         <v>159</v>
       </c>
       <c r="F8" s="4">
-        <f>100*E8/B8</f>
+        <f t="shared" si="0"/>
         <v>-4.032258064516129</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1361,7 +1394,7 @@
         <v>176</v>
       </c>
       <c r="L8" s="3">
-        <f>100*K8/B8</f>
+        <f t="shared" si="1"/>
         <v>-10.483870967741936</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1388,7 +1421,7 @@
         <v>166</v>
       </c>
       <c r="F9" s="4">
-        <f>100*E9/B9</f>
+        <f t="shared" si="0"/>
         <v>3.7865748709122204</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1407,7 +1440,7 @@
         <v>171</v>
       </c>
       <c r="L9" s="3">
-        <f>100*K9/B9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -1437,7 +1470,7 @@
         <v>162</v>
       </c>
       <c r="F10" s="4">
-        <f>100*E10/B10</f>
+        <f t="shared" si="0"/>
         <v>-2.4054982817869415</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1456,7 +1489,7 @@
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <f>100*K10/B10</f>
+        <f t="shared" si="1"/>
         <v>-6.8728522336769764</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -1483,7 +1516,7 @@
         <v>165</v>
       </c>
       <c r="F11" s="4">
-        <f>100*E11/B11</f>
+        <f t="shared" si="0"/>
         <v>6.3348416289592748</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1502,7 +1535,7 @@
         <v>181</v>
       </c>
       <c r="L11" s="3">
-        <f>100*K11/B11</f>
+        <f t="shared" si="1"/>
         <v>-18.099547511312217</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -1532,7 +1565,7 @@
         <v>164</v>
       </c>
       <c r="F12" s="4">
-        <f>100*E12/B12</f>
+        <f t="shared" si="0"/>
         <v>-2.7624309392265194</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1551,7 +1584,7 @@
         <v>180</v>
       </c>
       <c r="L12" s="3">
-        <f>100*K12/B12</f>
+        <f t="shared" si="1"/>
         <v>-17.127071823204417</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -1581,7 +1614,7 @@
         <v>171</v>
       </c>
       <c r="F13" s="4">
-        <f>100*E13/B13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1600,7 +1633,7 @@
         <v>171</v>
       </c>
       <c r="L13" s="3">
-        <f>100*K13/B13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -1630,7 +1663,7 @@
         <v>160</v>
       </c>
       <c r="F14" s="4">
-        <f>100*E14/B14</f>
+        <f t="shared" si="0"/>
         <v>-73.353293413173645</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1649,7 +1682,7 @@
         <v>171</v>
       </c>
       <c r="L14" s="3">
-        <f>100*K14/B14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -1676,7 +1709,7 @@
         <v>163</v>
       </c>
       <c r="F15" s="4">
-        <f>100*E15/B15</f>
+        <f t="shared" si="0"/>
         <v>-8.5409252669039155</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -1695,7 +1728,7 @@
         <v>171</v>
       </c>
       <c r="L15" s="3">
-        <f>100*K15/B15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -1725,7 +1758,7 @@
         <v>171</v>
       </c>
       <c r="F16" s="4">
-        <f>100*E16/B16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1744,7 +1777,7 @@
         <v>179</v>
       </c>
       <c r="L16" s="3">
-        <f>100*K16/B16</f>
+        <f t="shared" si="1"/>
         <v>-25.936599423631122</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -1774,7 +1807,7 @@
         <v>157</v>
       </c>
       <c r="F17" s="4">
-        <f>100*E17/B17</f>
+        <f t="shared" si="0"/>
         <v>-8.0246913580246915</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1793,7 +1826,7 @@
         <v>175</v>
       </c>
       <c r="L17" s="3">
-        <f>100*K17/B17</f>
+        <f t="shared" si="1"/>
         <v>-8.6419753086419746</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1820,7 +1853,7 @@
         <v>161</v>
       </c>
       <c r="F18" s="4">
-        <f>100*E18/B18</f>
+        <f t="shared" si="0"/>
         <v>-9.9255583126550881</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1839,7 +1872,7 @@
         <v>171</v>
       </c>
       <c r="L18" s="3">
-        <f>100*K18/B18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -1866,7 +1899,7 @@
         <v>171</v>
       </c>
       <c r="F19" s="4">
-        <f>100*E19/B19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1885,7 +1918,7 @@
         <v>171</v>
       </c>
       <c r="L19" s="3">
-        <f>100*K19/B19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -1905,4 +1938,912 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EC6A6D-4B86-4F3E-8B97-0DB1E7F3A4F8}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="15.81640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="4">
+        <f>100*D2/B2</f>
+        <v>-1.7766497461928934</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-6.0913705583756341</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="4">
+        <f>100*D3/B3</f>
+        <v>-1.1744966442953022</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-5.0335570469798663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="4">
+        <f>100*D4/B4</f>
+        <v>-2.0930232558139532</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" s="3">
+        <v>-5.8139534883720927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="4">
+        <f>100*D5/B5</f>
+        <v>-3.6458333333333335</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J5" s="3">
+        <v>-9.3749999999999982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A28C005-A024-49B1-8447-1BA8A60558B5}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.90625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="15.81640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20.90625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="26.1796875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" ref="E2:E15" si="0">100*D2/B2</f>
+        <v>-3.7854889589905363</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" s="3">
+        <f t="shared" ref="K2:K15" si="1">100*J2/B2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="232" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" si="1"/>
+        <v>-11.111111111111111</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.032258064516129</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>-10.483870967741936</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7865748709122204</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.4054982817869415</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>-6.8728522336769764</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>6.3348416289592748</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>-18.099547511312217</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.7624309392265194</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>-17.127071823204417</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="232" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>-73.353293413173645</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.5409252669039155</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>-25.936599423631122</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.0246913580246915</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.9255583126550881</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>